<commit_message>
Added rawdata preparation for the comparison of two children. Functionality is now working.
</commit_message>
<xml_diff>
--- a/test data/test data - boy.xlsx
+++ b/test data/test data - boy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deels\git\ChildrenPercentilePlot\test data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9ACE22F-9A26-4809-8433-7810B0EA2E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41DF1DF0-45DC-4183-8763-5BB64C0AAC8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rawdata" sheetId="1" r:id="rId1"/>
@@ -391,7 +391,7 @@
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -421,13 +421,13 @@
         <v>44635</v>
       </c>
       <c r="B2">
-        <v>4500</v>
+        <v>4600</v>
       </c>
       <c r="C2">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D2">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -435,7 +435,7 @@
         <v>44636</v>
       </c>
       <c r="B3">
-        <v>4160</v>
+        <v>4260</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -443,7 +443,7 @@
         <v>44637</v>
       </c>
       <c r="B4">
-        <v>4180</v>
+        <v>4280</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -451,7 +451,7 @@
         <v>44638</v>
       </c>
       <c r="B5">
-        <v>4190</v>
+        <v>4290</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -459,7 +459,7 @@
         <v>44639</v>
       </c>
       <c r="B6">
-        <v>4220</v>
+        <v>4320</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -467,7 +467,7 @@
         <v>44640</v>
       </c>
       <c r="B7">
-        <v>4300</v>
+        <v>4400</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -475,13 +475,13 @@
         <v>44641</v>
       </c>
       <c r="B8">
-        <v>4400</v>
+        <v>4500</v>
       </c>
       <c r="C8">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D8">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>